<commit_message>
fixing build error (24/12/2023)
</commit_message>
<xml_diff>
--- a/Personal projects/build-MyApp-Desktop_Qt_6_4_2_MinGW_64_bit-Debug/Data_source.xlsx
+++ b/Personal projects/build-MyApp-Desktop_Qt_6_4_2_MinGW_64_bit-Debug/Data_source.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="45">
   <si>
     <t>Tháng</t>
   </si>
@@ -148,6 +148,18 @@
   </si>
   <si>
     <t>dfgassg</t>
+  </si>
+  <si>
+    <t>456456</t>
+  </si>
+  <si>
+    <t>hfgh</t>
+  </si>
+  <si>
+    <t>65656756</t>
+  </si>
+  <si>
+    <t>rthgfhfghfgh</t>
   </si>
 </sst>
 </file>
@@ -1189,13 +1201,13 @@
         <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G7" s="8">
         <v>21</v>
@@ -1285,13 +1297,13 @@
         <v>28</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>26</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>